<commit_message>
Final update before pre-scan 1
Cleared folder so it was smaller, moved results to C;\fmri for later analysis.
</commit_message>
<xml_diff>
--- a/docs/per_pre_counterbalance.xlsx
+++ b/docs/per_pre_counterbalance.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="23190" windowHeight="10695" activeTab="2"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="23190" windowHeight="10695" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -209,1217 +209,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="129">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1778,7 +568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L3" sqref="L3:S21"/>
     </sheetView>
   </sheetViews>
@@ -3363,17 +2153,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:J23">
-    <cfRule type="cellIs" dxfId="128" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:J10">
-    <cfRule type="cellIs" dxfId="127" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:J23">
-    <cfRule type="cellIs" dxfId="126" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3385,7 +2175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
@@ -4667,7 +3457,7 @@
         <v>12</v>
       </c>
       <c r="I22" s="8">
-        <f t="shared" ref="I22:P22" si="14">SUM(I12:I21)</f>
+        <f t="shared" ref="I22:L22" si="14">SUM(I12:I21)</f>
         <v>12</v>
       </c>
       <c r="J22" s="3">
@@ -4683,35 +3473,35 @@
         <v>12</v>
       </c>
       <c r="M22" s="8">
-        <f>SUM(M12:M21)</f>
+        <f t="shared" ref="M22:T22" si="15">SUM(M12:M21)</f>
         <v>12</v>
       </c>
       <c r="N22" s="3">
-        <f>SUM(N12:N21)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="O22" s="3">
-        <f>SUM(O12:O21)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="P22" s="2">
-        <f>SUM(P12:P21)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="Q22" s="8">
-        <f>SUM(Q12:Q21)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="R22" s="3">
-        <f>SUM(R12:R21)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="S22" s="3">
-        <f>SUM(S12:S21)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="T22" s="2">
-        <f>SUM(T12:T21)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
     </row>
@@ -4721,15 +3511,15 @@
         <v>34</v>
       </c>
       <c r="B23" s="6">
-        <f t="shared" ref="B23:D23" si="15">B1+B12</f>
+        <f t="shared" ref="B23:D23" si="16">B1+B12</f>
         <v>5</v>
       </c>
       <c r="C23" s="6">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="D23" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="E23" s="5">
@@ -4737,15 +3527,15 @@
         <v>24</v>
       </c>
       <c r="F23" s="6">
-        <f t="shared" ref="F23:H23" si="16">F1+F12</f>
+        <f t="shared" ref="F23:H23" si="17">F1+F12</f>
         <v>30</v>
       </c>
       <c r="G23" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>16</v>
       </c>
       <c r="H23" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>17</v>
       </c>
       <c r="I23" s="5">
@@ -4753,15 +3543,15 @@
         <v>33</v>
       </c>
       <c r="J23" s="6">
-        <f t="shared" ref="J23:L23" si="17">J1+J12</f>
+        <f t="shared" ref="J23:L23" si="18">J1+J12</f>
         <v>28</v>
       </c>
       <c r="K23" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>30</v>
       </c>
       <c r="L23" s="6">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>21</v>
       </c>
       <c r="M23" s="5">
@@ -4769,15 +3559,15 @@
         <v>11</v>
       </c>
       <c r="N23" s="6">
-        <f t="shared" ref="N23:P23" si="18">N1+N12</f>
+        <f t="shared" ref="N23:P23" si="19">N1+N12</f>
         <v>13</v>
       </c>
       <c r="O23" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>18</v>
       </c>
       <c r="P23" s="6">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>34</v>
       </c>
       <c r="Q23" s="5">
@@ -4785,69 +3575,69 @@
         <v>6</v>
       </c>
       <c r="R23" s="6">
-        <f t="shared" ref="R23:T23" si="19">R12+R1</f>
+        <f t="shared" ref="R23:T23" si="20">R12+R1</f>
         <v>33</v>
       </c>
       <c r="S23" s="6">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>27</v>
       </c>
       <c r="T23" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f t="shared" ref="A24:H24" si="20">A2+A13</f>
+        <f t="shared" ref="A24:H24" si="21">A2+A13</f>
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>34</v>
       </c>
       <c r="E24" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>33</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>21</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>32</v>
       </c>
       <c r="I24" s="8">
-        <f t="shared" ref="I24:M24" si="21">I2+I13</f>
+        <f t="shared" ref="I24:M24" si="22">I2+I13</f>
         <v>6</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>13</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>8</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>11</v>
       </c>
       <c r="M24" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>34</v>
       </c>
       <c r="N24" s="1">
@@ -4855,15 +3645,15 @@
         <v>24</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" ref="N24:P24" si="22">O2+O13</f>
+        <f t="shared" ref="O24:P24" si="23">O2+O13</f>
         <v>2</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>33</v>
       </c>
       <c r="Q24" s="8">
-        <f t="shared" ref="Q24:Q32" si="23">Q13+Q2</f>
+        <f t="shared" ref="Q24:Q32" si="24">Q13+Q2</f>
         <v>16</v>
       </c>
       <c r="R24" s="1">
@@ -4875,221 +3665,221 @@
         <v>20</v>
       </c>
       <c r="T24" s="2">
-        <f t="shared" ref="T24" si="24">T13+T2</f>
+        <f t="shared" ref="T24" si="25">T13+T2</f>
         <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f t="shared" ref="A25:H25" si="25">A3+A14</f>
+        <f t="shared" ref="A25:H25" si="26">A3+A14</f>
         <v>30</v>
       </c>
       <c r="B25" s="1">
-        <f t="shared" si="25"/>
-        <v>26</v>
-      </c>
-      <c r="C25" s="1">
-        <f t="shared" si="25"/>
-        <v>34</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="25"/>
-        <v>24</v>
-      </c>
-      <c r="E25" s="8">
-        <f t="shared" si="25"/>
-        <v>6</v>
-      </c>
-      <c r="F25" s="1">
-        <f t="shared" si="25"/>
-        <v>4</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" si="25"/>
-        <v>33</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" si="25"/>
-        <v>15</v>
-      </c>
-      <c r="I25" s="8">
-        <f t="shared" ref="I25:M25" si="26">I3+I14</f>
-        <v>12</v>
-      </c>
-      <c r="J25" s="1">
-        <f t="shared" si="26"/>
-        <v>19</v>
-      </c>
-      <c r="K25" s="1">
-        <f t="shared" si="26"/>
-        <v>34</v>
-      </c>
-      <c r="L25" s="1">
         <f t="shared" si="26"/>
         <v>26</v>
       </c>
+      <c r="C25" s="1">
+        <f t="shared" si="26"/>
+        <v>34</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="26"/>
+        <v>24</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="26"/>
+        <v>4</v>
+      </c>
+      <c r="G25" s="1">
+        <f t="shared" si="26"/>
+        <v>33</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="26"/>
+        <v>15</v>
+      </c>
+      <c r="I25" s="8">
+        <f t="shared" ref="I25:M25" si="27">I3+I14</f>
+        <v>12</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="27"/>
+        <v>19</v>
+      </c>
+      <c r="K25" s="1">
+        <f t="shared" si="27"/>
+        <v>34</v>
+      </c>
+      <c r="L25" s="1">
+        <f t="shared" si="27"/>
+        <v>26</v>
+      </c>
       <c r="M25" s="8">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>33</v>
       </c>
       <c r="N25" s="1">
-        <f t="shared" ref="N25:P25" si="27">N3+N14</f>
+        <f t="shared" ref="N25:P25" si="28">N3+N14</f>
         <v>1</v>
       </c>
       <c r="O25" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>7</v>
       </c>
       <c r="P25" s="1">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>17</v>
       </c>
       <c r="Q25" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>18</v>
       </c>
       <c r="R25" s="1">
-        <f t="shared" ref="R25:T25" si="28">R14+R3</f>
+        <f t="shared" ref="R25:T25" si="29">R14+R3</f>
         <v>24</v>
       </c>
       <c r="S25" s="1">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>32</v>
       </c>
       <c r="T25" s="2">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <f t="shared" ref="A26:H26" si="29">A4+A15</f>
+        <f t="shared" ref="A26:H26" si="30">A4+A15</f>
         <v>8</v>
       </c>
       <c r="B26" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>23</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>19</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>27</v>
       </c>
       <c r="E26" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>10</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>33</v>
       </c>
       <c r="G26" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>31</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="I26" s="8">
-        <f t="shared" ref="I26:M26" si="30">I4+I15</f>
+        <f t="shared" ref="I26:M26" si="31">I4+I15</f>
         <v>14</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>34</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>9</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>33</v>
       </c>
       <c r="M26" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>8</v>
       </c>
       <c r="N26" s="1">
-        <f t="shared" ref="N26:P26" si="31">N4+N15</f>
+        <f t="shared" ref="N26:P26" si="32">N4+N15</f>
         <v>20</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>28</v>
       </c>
       <c r="P26" s="1">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="Q26" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>31</v>
       </c>
       <c r="R26" s="1">
-        <f t="shared" ref="R26:T26" si="32">R15+R4</f>
+        <f t="shared" ref="R26:T26" si="33">R15+R4</f>
         <v>15</v>
       </c>
       <c r="S26" s="1">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>21</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <f t="shared" ref="A27:H27" si="33">A5+A16</f>
+        <f t="shared" ref="A27:H27" si="34">A5+A16</f>
         <v>17</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>34</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>6</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="E27" s="8">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>13</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>28</v>
       </c>
       <c r="G27" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>12</v>
       </c>
       <c r="H27" s="2">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>22</v>
       </c>
       <c r="I27" s="8">
-        <f t="shared" ref="I27:M27" si="34">I5+I16</f>
+        <f t="shared" ref="I27:L27" si="35">I5+I16</f>
         <v>29</v>
       </c>
       <c r="J27" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>33</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>18</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>32</v>
       </c>
       <c r="M27" s="8">
@@ -5097,179 +3887,179 @@
         <v>14</v>
       </c>
       <c r="N27" s="1">
-        <f t="shared" ref="N27:P27" si="35">N5+N16</f>
+        <f t="shared" ref="N27:P27" si="36">N5+N16</f>
         <v>10</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>33</v>
       </c>
       <c r="P27" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>22</v>
       </c>
       <c r="Q27" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>25</v>
       </c>
       <c r="R27" s="1">
-        <f t="shared" ref="R27:T27" si="36">R16+R5</f>
+        <f t="shared" ref="R27:T27" si="37">R16+R5</f>
         <v>34</v>
       </c>
       <c r="S27" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>2</v>
       </c>
       <c r="T27" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <f t="shared" ref="A28:H28" si="37">A6+A17</f>
+        <f t="shared" ref="A28:H28" si="38">A6+A17</f>
         <v>16</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>31</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>28</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>7</v>
       </c>
       <c r="E28" s="8">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>34</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>9</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>23</v>
       </c>
       <c r="H28" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>33</v>
       </c>
       <c r="I28" s="8">
-        <f t="shared" ref="I28:M28" si="38">I6+I17</f>
+        <f t="shared" ref="I28:M28" si="39">I6+I17</f>
         <v>20</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>4</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>34</v>
       </c>
       <c r="M28" s="8">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>19</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" ref="N28:P28" si="39">N6+N17</f>
+        <f t="shared" ref="N28:P28" si="40">N6+N17</f>
         <v>27</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>29</v>
       </c>
       <c r="P28" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>5</v>
       </c>
       <c r="Q28" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>23</v>
       </c>
       <c r="R28" s="1">
-        <f t="shared" ref="R28:T28" si="40">R17+R6</f>
+        <f t="shared" ref="R28:T28" si="41">R17+R6</f>
         <v>10</v>
       </c>
       <c r="S28" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>14</v>
       </c>
       <c r="T28" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <f t="shared" ref="A29:H29" si="41">A7+A18</f>
+        <f t="shared" ref="A29:H29" si="42">A7+A18</f>
         <v>22</v>
       </c>
       <c r="B29" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>13</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>33</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>18</v>
       </c>
       <c r="E29" s="8">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>27</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>34</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>5</v>
       </c>
       <c r="H29" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>11</v>
       </c>
       <c r="I29" s="8">
-        <f t="shared" ref="I29:M29" si="42">I7+I18</f>
+        <f t="shared" ref="I29:M29" si="43">I7+I18</f>
         <v>3</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>31</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>24</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>16</v>
       </c>
       <c r="M29" s="8">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>25</v>
       </c>
       <c r="N29" s="1">
-        <f t="shared" ref="N29:P29" si="43">N7+N18</f>
+        <f t="shared" ref="N29:P29" si="44">N7+N18</f>
         <v>33</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>34</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>32</v>
       </c>
       <c r="Q29" s="8">
@@ -5277,77 +4067,77 @@
         <v>4</v>
       </c>
       <c r="R29" s="1">
-        <f t="shared" ref="R29:T29" si="44">R18+R7</f>
+        <f t="shared" ref="R29:T29" si="45">R18+R7</f>
         <v>17</v>
       </c>
       <c r="S29" s="1">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>5</v>
       </c>
       <c r="T29" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <f t="shared" ref="A30:H30" si="45">A8+A19</f>
+        <f t="shared" ref="A30:H30" si="46">A8+A19</f>
         <v>11</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>4</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>32</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>33</v>
       </c>
       <c r="E30" s="8">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>20</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>14</v>
       </c>
       <c r="G30" s="1">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>34</v>
       </c>
       <c r="H30" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>8</v>
       </c>
       <c r="I30" s="8">
-        <f t="shared" ref="I30:M30" si="46">I8+I19</f>
+        <f t="shared" ref="I30:M30" si="47">I8+I19</f>
         <v>25</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>22</v>
       </c>
       <c r="K30" s="1">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>33</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>7</v>
       </c>
       <c r="M30" s="8">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>30</v>
       </c>
       <c r="N30" s="1">
-        <f t="shared" ref="N30:P30" si="47">N8+N19</f>
+        <f t="shared" ref="N30:O30" si="48">N8+N19</f>
         <v>34</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>9</v>
       </c>
       <c r="P30" s="1">
@@ -5355,19 +4145,19 @@
         <v>15</v>
       </c>
       <c r="Q30" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>33</v>
       </c>
       <c r="R30" s="1">
-        <f t="shared" ref="R30:T30" si="48">R19+R8</f>
+        <f t="shared" ref="R30:T30" si="49">R19+R8</f>
         <v>3</v>
       </c>
       <c r="S30" s="1">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>11</v>
       </c>
       <c r="T30" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>22</v>
       </c>
     </row>
@@ -5377,55 +4167,55 @@
         <v>3</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" ref="B31:H31" si="49">B9+B20</f>
+        <f t="shared" ref="B31:H31" si="50">B9+B20</f>
         <v>33</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>21</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>14</v>
       </c>
       <c r="E31" s="8">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>29</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>7</v>
       </c>
       <c r="G31" s="1">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>18</v>
       </c>
       <c r="H31" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>26</v>
       </c>
       <c r="I31" s="8">
-        <f t="shared" ref="I31:M31" si="50">I9+I20</f>
+        <f t="shared" ref="I31:M31" si="51">I9+I20</f>
         <v>34</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>10</v>
       </c>
       <c r="K31" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>15</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>17</v>
       </c>
       <c r="M31" s="8">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>4</v>
       </c>
       <c r="N31" s="1">
-        <f t="shared" ref="N31:P31" si="51">N9+N20</f>
+        <f t="shared" ref="N31:P31" si="52">N9+N20</f>
         <v>31</v>
       </c>
       <c r="O31" s="1">
@@ -5433,105 +4223,105 @@
         <v>23</v>
       </c>
       <c r="P31" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>26</v>
       </c>
       <c r="Q31" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>9</v>
       </c>
       <c r="R31" s="1">
-        <f t="shared" ref="R31:T31" si="52">R20+R9</f>
+        <f t="shared" ref="R31:T31" si="53">R20+R9</f>
         <v>8</v>
       </c>
       <c r="S31" s="1">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>34</v>
       </c>
       <c r="T31" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
-        <f t="shared" ref="A32:H32" si="53">A10+A21</f>
+        <f t="shared" ref="A32:H32" si="54">A10+A21</f>
         <v>33</v>
       </c>
       <c r="B32" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>10</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>15</v>
       </c>
       <c r="D32" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>29</v>
       </c>
       <c r="E32" s="9">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>3</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>19</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>25</v>
       </c>
       <c r="H32" s="10">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>34</v>
       </c>
       <c r="I32" s="9">
-        <f t="shared" ref="I32:M32" si="54">I10+I21</f>
+        <f t="shared" ref="I32:M32" si="55">I10+I21</f>
         <v>23</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>5</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>27</v>
       </c>
       <c r="L32" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>2</v>
       </c>
       <c r="M32" s="9">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>21</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" ref="N32:P32" si="55">N10+N21</f>
+        <f t="shared" ref="N32:P32" si="56">N10+N21</f>
         <v>6</v>
       </c>
       <c r="O32" s="4">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>16</v>
       </c>
       <c r="P32" s="4">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>12</v>
       </c>
       <c r="Q32" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>34</v>
       </c>
       <c r="R32" s="4">
-        <f t="shared" ref="R32:T32" si="56">R21+R10</f>
+        <f t="shared" ref="R32:T32" si="57">R21+R10</f>
         <v>29</v>
       </c>
       <c r="S32" s="4">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>33</v>
       </c>
       <c r="T32" s="10">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>19</v>
       </c>
     </row>
@@ -5559,17 +4349,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:P10">
-    <cfRule type="cellIs" dxfId="10" priority="71" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="71" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:J10">
-    <cfRule type="cellIs" dxfId="9" priority="70" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="70" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:P10">
-    <cfRule type="cellIs" dxfId="8" priority="67" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="67" operator="greaterThan">
       <formula>34</formula>
     </cfRule>
     <cfRule type="colorScale" priority="68">
@@ -5668,7 +4458,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:H10">
-    <cfRule type="cellIs" dxfId="7" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="21" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
     <cfRule type="colorScale" priority="20">
@@ -5683,7 +4473,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q1:T10">
-    <cfRule type="cellIs" dxfId="6" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="19" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
     <cfRule type="colorScale" priority="18">

</xml_diff>